<commit_message>
add search box in /mylist
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/tempxls/개발테스트.xlsx
+++ b/src/main/webapp/resources/tempxls/개발테스트.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="206">
   <si>
     <t>LGIT P/N</t>
   </si>
@@ -83,6 +83,39 @@
     <t>출고시험용</t>
   </si>
   <si>
+    <t>AAAdSLDKJF</t>
+  </si>
+  <si>
+    <t>GLKLVNBDM</t>
+  </si>
+  <si>
+    <t>ei399</t>
+  </si>
+  <si>
+    <t>창고앞</t>
+  </si>
+  <si>
+    <t>!@$-011</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>TESTPRJA1</t>
+  </si>
+  <si>
+    <t>TESTPRJA2</t>
+  </si>
+  <si>
+    <t>TESTPRJA3</t>
+  </si>
+  <si>
+    <t>창고뒤A</t>
+  </si>
+  <si>
+    <t>GESS</t>
+  </si>
+  <si>
     <t>AGAINEESS</t>
   </si>
   <si>
@@ -92,45 +125,51 @@
     <t>399fdkAA</t>
   </si>
   <si>
+    <t>3층A사이드</t>
+  </si>
+  <si>
+    <t>GDFWEF</t>
+  </si>
+  <si>
+    <t>AGAINNEWAA</t>
+  </si>
+  <si>
+    <t>39fjdn2AA</t>
+  </si>
+  <si>
+    <t>MMGG</t>
+  </si>
+  <si>
+    <t>L432</t>
+  </si>
+  <si>
+    <t>GGEE</t>
+  </si>
+  <si>
+    <t>NEWEXCELIM</t>
+  </si>
+  <si>
+    <t>Hdidlfkje</t>
+  </si>
+  <si>
+    <t>384+2124</t>
+  </si>
+  <si>
+    <t>LG19281NN</t>
+  </si>
+  <si>
+    <t>Desdkfkdfjk</t>
+  </si>
+  <si>
+    <t>MMMMAAAAABB</t>
+  </si>
+  <si>
     <t>loapdlkj111</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>AGAINNEWAA</t>
-  </si>
-  <si>
-    <t>39fjdn2AA</t>
-  </si>
-  <si>
-    <t>MMGG</t>
-  </si>
-  <si>
-    <t>L432</t>
-  </si>
-  <si>
-    <t>384+2124</t>
-  </si>
-  <si>
-    <t>NEWEXCELIM</t>
-  </si>
-  <si>
-    <t>Hdidlfkje</t>
-  </si>
-  <si>
-    <t>LG19281NN</t>
-  </si>
-  <si>
-    <t>Desdkfkdfjk</t>
-  </si>
-  <si>
-    <t>MMMMAAAAABB</t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
@@ -158,36 +197,39 @@
     <t>GRM0335C1H2R5BA01</t>
   </si>
   <si>
+    <t>GGGE</t>
+  </si>
+  <si>
+    <t>2CAC01187A</t>
+  </si>
+  <si>
+    <t>GRM0335C1HR60WA01</t>
+  </si>
+  <si>
+    <t>G122</t>
+  </si>
+  <si>
+    <t>2LL2N7BA11K-H</t>
+  </si>
+  <si>
+    <t>LQP03TN2N7B02D</t>
+  </si>
+  <si>
+    <t>G555</t>
+  </si>
+  <si>
+    <t>2DIT00095A</t>
+  </si>
+  <si>
+    <t>VCUT05E1-SD0</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
     <t>20+-20</t>
   </si>
   <si>
-    <t>2CAC01187A</t>
-  </si>
-  <si>
-    <t>GRM0335C1HR60WA01</t>
-  </si>
-  <si>
-    <t>2LL2N7BA11K-H</t>
-  </si>
-  <si>
-    <t>LQP03TN2N7B02D</t>
-  </si>
-  <si>
-    <t>2FTS00105A</t>
-  </si>
-  <si>
-    <t>SAFFB806MFA0F1B</t>
-  </si>
-  <si>
-    <t>2DIT00095A</t>
-  </si>
-  <si>
-    <t>VCUT05E1-SD0</t>
-  </si>
-  <si>
-    <t>Vishay</t>
-  </si>
-  <si>
     <t>2FTZ00032A</t>
   </si>
   <si>
@@ -203,18 +245,15 @@
     <t>SAWFD1G84BH0F0A</t>
   </si>
   <si>
+    <t>20+-2011</t>
+  </si>
+  <si>
     <t>2LL3N4BA11K-R</t>
   </si>
   <si>
     <t>LQP03TN3N4B02D</t>
   </si>
   <si>
-    <t>2LL3N2BA11K-H</t>
-  </si>
-  <si>
-    <t>LQP03TN3N2B02D</t>
-  </si>
-  <si>
     <t>2ICL00079A</t>
   </si>
   <si>
@@ -309,27 +348,6 @@
   </si>
   <si>
     <t>MAGLAYERS</t>
-  </si>
-  <si>
-    <t>2FTS00096A</t>
-  </si>
-  <si>
-    <t>F6HF2G441AF46</t>
-  </si>
-  <si>
-    <t>2FTS00093A</t>
-  </si>
-  <si>
-    <t>B39242-B4346-P810</t>
-  </si>
-  <si>
-    <t>EPCOS AG</t>
-  </si>
-  <si>
-    <t>2FTC00145A</t>
-  </si>
-  <si>
-    <t>DLU-2012-25GS1-A1-AT</t>
   </si>
   <si>
     <t>2FTP00015A</t>
@@ -1203,10 +1221,10 @@
         <v>20</v>
       </c>
       <c r="H5" t="n">
-        <v>123.02300262451172</v>
+        <v>54.540000915527344</v>
       </c>
       <c r="I5" t="n">
-        <v>50.0</v>
+        <v>998.0</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -1241,10 +1259,10 @@
         <v>26</v>
       </c>
       <c r="H6" t="n">
-        <v>55.0</v>
+        <v>23.239999771118164</v>
       </c>
       <c r="I6" t="n">
-        <v>1072.0</v>
+        <v>997.0</v>
       </c>
       <c r="J6" t="s">
         <v>27</v>
@@ -1276,19 +1294,19 @@
         <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H7" t="n">
-        <v>55.0</v>
+        <v>21.547000885009766</v>
       </c>
       <c r="I7" t="n">
-        <v>1075.0</v>
+        <v>888.0</v>
       </c>
       <c r="J7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
@@ -1308,25 +1326,25 @@
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H8" t="n">
-        <v>123.0</v>
+        <v>123457.0</v>
       </c>
       <c r="I8" t="n">
-        <v>486.0</v>
+        <v>88.0</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="K8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L8" t="s">
         <v>23</v>
@@ -1346,25 +1364,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H9" t="n">
-        <v>123.0</v>
+        <v>123456.0</v>
       </c>
       <c r="I9" t="n">
-        <v>123.0</v>
+        <v>77.0</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="L9" t="s">
         <v>23</v>
@@ -1384,25 +1402,25 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="H10" t="n">
-        <v>0.10000000149011612</v>
+        <v>5.656400203704834</v>
       </c>
       <c r="I10" t="n">
-        <v>150.0</v>
+        <v>789.0</v>
       </c>
       <c r="J10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>
@@ -1422,25 +1440,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H11" t="n">
-        <v>0.10000000149011612</v>
+        <v>77.0</v>
       </c>
       <c r="I11" t="n">
-        <v>9740.0</v>
+        <v>123.0</v>
       </c>
       <c r="J11" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="L11" t="s">
         <v>23</v>
@@ -1460,25 +1478,25 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H12" t="n">
-        <v>0.10000000149011612</v>
+        <v>88.0</v>
       </c>
       <c r="I12" t="n">
-        <v>9975.0</v>
+        <v>150.0</v>
       </c>
       <c r="J12" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="L12" t="s">
         <v>23</v>
@@ -1498,25 +1516,25 @@
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H13" t="n">
-        <v>0.10000000149011612</v>
+        <v>99.0</v>
       </c>
       <c r="I13" t="n">
-        <v>1934.0</v>
+        <v>97545.0</v>
       </c>
       <c r="J13" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="L13" t="s">
         <v>23</v>
@@ -1536,25 +1554,25 @@
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H14" t="n">
-        <v>0.10000000149011612</v>
+        <v>100.0</v>
       </c>
       <c r="I14" t="n">
-        <v>1950.0</v>
+        <v>9975.0</v>
       </c>
       <c r="J14" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K14" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="L14" t="s">
         <v>23</v>
@@ -1574,25 +1592,25 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I15" t="n">
-        <v>12600.0</v>
+        <v>1934.0</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="L15" t="s">
         <v>23</v>
@@ -1612,25 +1630,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="H16" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I16" t="n">
-        <v>510.0</v>
+        <v>12600.0</v>
       </c>
       <c r="J16" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K16" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L16" t="s">
         <v>23</v>
@@ -1650,25 +1668,25 @@
         <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="H17" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I17" t="n">
-        <v>4247.0</v>
+        <v>510.0</v>
       </c>
       <c r="J17" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K17" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L17" t="s">
         <v>23</v>
@@ -1688,25 +1706,25 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H18" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I18" t="n">
-        <v>2930.0</v>
+        <v>4247.0</v>
       </c>
       <c r="J18" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K18" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="L18" t="s">
         <v>23</v>
@@ -1726,25 +1744,25 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H19" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I19" t="n">
-        <v>7260.0</v>
+        <v>2930.0</v>
       </c>
       <c r="J19" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K19" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
@@ -1764,13 +1782,13 @@
         <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="H20" t="n">
         <v>0.10000000149011612</v>
@@ -1779,10 +1797,10 @@
         <v>2200.0</v>
       </c>
       <c r="J20" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K20" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L20" t="s">
         <v>23</v>
@@ -1802,13 +1820,13 @@
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H21" t="n">
         <v>0.10000000149011612</v>
@@ -1817,10 +1835,10 @@
         <v>2127.0</v>
       </c>
       <c r="J21" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K21" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
@@ -1840,13 +1858,13 @@
         <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H22" t="n">
         <v>0.10000000149011612</v>
@@ -1855,10 +1873,10 @@
         <v>2170.0</v>
       </c>
       <c r="J22" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K22" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L22" t="s">
         <v>23</v>
@@ -1878,13 +1896,13 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F23" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="G23" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H23" t="n">
         <v>0.10000000149011612</v>
@@ -1893,10 +1911,10 @@
         <v>2180.0</v>
       </c>
       <c r="J23" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K23" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
@@ -1916,13 +1934,13 @@
         <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H24" t="n">
         <v>0.10000000149011612</v>
@@ -1931,10 +1949,10 @@
         <v>1670.0</v>
       </c>
       <c r="J24" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K24" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L24" t="s">
         <v>23</v>
@@ -1954,13 +1972,13 @@
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H25" t="n">
         <v>0.10000000149011612</v>
@@ -1969,10 +1987,10 @@
         <v>1712.0</v>
       </c>
       <c r="J25" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K25" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L25" t="s">
         <v>23</v>
@@ -1992,13 +2010,13 @@
         <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F26" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="G26" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H26" t="n">
         <v>0.10000000149011612</v>
@@ -2007,10 +2025,10 @@
         <v>1680.0</v>
       </c>
       <c r="J26" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K26" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L26" t="s">
         <v>23</v>
@@ -2030,13 +2048,13 @@
         <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="F27" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H27" t="n">
         <v>0.10000000149011612</v>
@@ -2045,10 +2063,10 @@
         <v>1610.0</v>
       </c>
       <c r="J27" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K27" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L27" t="s">
         <v>23</v>
@@ -2068,13 +2086,13 @@
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F28" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="G28" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="H28" t="n">
         <v>0.10000000149011612</v>
@@ -2083,10 +2101,10 @@
         <v>1650.0</v>
       </c>
       <c r="J28" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K28" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L28" t="s">
         <v>23</v>
@@ -2106,13 +2124,13 @@
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="G29" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H29" t="n">
         <v>0.10000000149011612</v>
@@ -2121,10 +2139,10 @@
         <v>3660.0</v>
       </c>
       <c r="J29" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K29" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L29" t="s">
         <v>23</v>
@@ -2144,13 +2162,13 @@
         <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H30" t="n">
         <v>0.10000000149011612</v>
@@ -2159,10 +2177,10 @@
         <v>3790.0</v>
       </c>
       <c r="J30" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K30" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L30" t="s">
         <v>23</v>
@@ -2182,13 +2200,13 @@
         <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="F31" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="G31" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H31" t="n">
         <v>0.10000000149011612</v>
@@ -2197,10 +2215,10 @@
         <v>4300.0</v>
       </c>
       <c r="J31" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K31" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L31" t="s">
         <v>23</v>
@@ -2220,13 +2238,13 @@
         <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="F32" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="G32" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="H32" t="n">
         <v>0.10000000149011612</v>
@@ -2235,10 +2253,10 @@
         <v>8980.0</v>
       </c>
       <c r="J32" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K32" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L32" t="s">
         <v>23</v>
@@ -2258,25 +2276,25 @@
         <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="F33" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="G33" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="H33" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I33" t="n">
-        <v>4480.0</v>
+        <v>4447.0</v>
       </c>
       <c r="J33" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K33" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L33" t="s">
         <v>23</v>
@@ -2296,25 +2314,25 @@
         <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="G34" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H34" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I34" t="n">
-        <v>530.0</v>
+        <v>2260.0</v>
       </c>
       <c r="J34" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K34" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L34" t="s">
         <v>23</v>
@@ -2334,25 +2352,25 @@
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="F35" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="H35" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I35" t="n">
-        <v>3000.0</v>
+        <v>768.0</v>
       </c>
       <c r="J35" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K35" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L35" t="s">
         <v>23</v>
@@ -2372,25 +2390,25 @@
         <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="F36" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="G36" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="H36" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I36" t="n">
-        <v>4450.0</v>
+        <v>1275.0</v>
       </c>
       <c r="J36" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K36" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L36" t="s">
         <v>23</v>
@@ -2410,25 +2428,25 @@
         <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="F37" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="G37" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="H37" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I37" t="n">
-        <v>2260.0</v>
+        <v>2200.0</v>
       </c>
       <c r="J37" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K37" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L37" t="s">
         <v>23</v>
@@ -2448,25 +2466,25 @@
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="F38" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="G38" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="H38" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I38" t="n">
-        <v>768.0</v>
+        <v>1560.0</v>
       </c>
       <c r="J38" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K38" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L38" t="s">
         <v>23</v>
@@ -2486,25 +2504,25 @@
         <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="F39" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="G39" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="H39" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I39" t="n">
-        <v>1275.0</v>
+        <v>1330.0</v>
       </c>
       <c r="J39" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K39" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L39" t="s">
         <v>23</v>
@@ -2524,25 +2542,25 @@
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="F40" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="G40" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="H40" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I40" t="n">
-        <v>2200.0</v>
+        <v>1330.0</v>
       </c>
       <c r="J40" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K40" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L40" t="s">
         <v>23</v>
@@ -2562,25 +2580,25 @@
         <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="F41" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="G41" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H41" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I41" t="n">
-        <v>1560.0</v>
+        <v>1020.0</v>
       </c>
       <c r="J41" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K41" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L41" t="s">
         <v>23</v>
@@ -2600,25 +2618,25 @@
         <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="F42" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="G42" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H42" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I42" t="n">
-        <v>1330.0</v>
+        <v>15830.0</v>
       </c>
       <c r="J42" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K42" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L42" t="s">
         <v>23</v>
@@ -2638,25 +2656,25 @@
         <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="F43" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="H43" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I43" t="n">
-        <v>1330.0</v>
+        <v>500.0</v>
       </c>
       <c r="J43" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K43" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L43" t="s">
         <v>23</v>
@@ -2676,25 +2694,25 @@
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="F44" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="G44" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H44" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I44" t="n">
-        <v>1020.0</v>
+        <v>19.0</v>
       </c>
       <c r="J44" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K44" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L44" t="s">
         <v>23</v>
@@ -2714,25 +2732,25 @@
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="F45" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G45" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H45" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I45" t="n">
-        <v>15830.0</v>
+        <v>2710.0</v>
       </c>
       <c r="J45" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K45" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L45" t="s">
         <v>23</v>
@@ -2752,25 +2770,25 @@
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="F46" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="G46" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="H46" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I46" t="n">
-        <v>500.0</v>
+        <v>187.0</v>
       </c>
       <c r="J46" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K46" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L46" t="s">
         <v>23</v>
@@ -2790,25 +2808,25 @@
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="F47" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="G47" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H47" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I47" t="n">
-        <v>19.0</v>
+        <v>680.0</v>
       </c>
       <c r="J47" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K47" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L47" t="s">
         <v>23</v>
@@ -2828,25 +2846,25 @@
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="F48" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="G48" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="H48" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I48" t="n">
-        <v>2710.0</v>
+        <v>72.0</v>
       </c>
       <c r="J48" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K48" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L48" t="s">
         <v>23</v>
@@ -2866,25 +2884,25 @@
         <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="F49" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="G49" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="H49" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I49" t="n">
-        <v>187.0</v>
+        <v>4060.0</v>
       </c>
       <c r="J49" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K49" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L49" t="s">
         <v>23</v>
@@ -2904,25 +2922,25 @@
         <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F50" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="G50" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="H50" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I50" t="n">
-        <v>680.0</v>
+        <v>520.0</v>
       </c>
       <c r="J50" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K50" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L50" t="s">
         <v>23</v>
@@ -2942,25 +2960,25 @@
         <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="F51" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="G51" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="H51" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I51" t="n">
-        <v>72.0</v>
+        <v>520.0</v>
       </c>
       <c r="J51" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K51" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L51" t="s">
         <v>23</v>
@@ -2980,25 +2998,25 @@
         <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="F52" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="G52" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H52" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I52" t="n">
-        <v>4060.0</v>
+        <v>3300.0</v>
       </c>
       <c r="J52" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K52" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L52" t="s">
         <v>23</v>
@@ -3018,25 +3036,25 @@
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="F53" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="G53" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H53" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I53" t="n">
-        <v>520.0</v>
+        <v>530.0</v>
       </c>
       <c r="J53" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K53" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L53" t="s">
         <v>23</v>
@@ -3056,25 +3074,25 @@
         <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="F54" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="G54" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H54" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I54" t="n">
-        <v>520.0</v>
+        <v>1270.0</v>
       </c>
       <c r="J54" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K54" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L54" t="s">
         <v>23</v>
@@ -3094,25 +3112,25 @@
         <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="F55" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="G55" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H55" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I55" t="n">
-        <v>3300.0</v>
+        <v>1430.0</v>
       </c>
       <c r="J55" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K55" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L55" t="s">
         <v>23</v>
@@ -3132,25 +3150,25 @@
         <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="F56" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="G56" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H56" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I56" t="n">
-        <v>530.0</v>
+        <v>480.0</v>
       </c>
       <c r="J56" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K56" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L56" t="s">
         <v>23</v>
@@ -3170,25 +3188,25 @@
         <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="F57" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="G57" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H57" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I57" t="n">
-        <v>1270.0</v>
+        <v>530.0</v>
       </c>
       <c r="J57" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K57" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L57" t="s">
         <v>23</v>
@@ -3208,25 +3226,25 @@
         <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="F58" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="G58" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H58" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I58" t="n">
-        <v>1430.0</v>
+        <v>530.0</v>
       </c>
       <c r="J58" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K58" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L58" t="s">
         <v>23</v>
@@ -3246,25 +3264,25 @@
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="F59" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G59" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H59" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I59" t="n">
-        <v>480.0</v>
+        <v>510.0</v>
       </c>
       <c r="J59" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K59" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L59" t="s">
         <v>23</v>
@@ -3284,25 +3302,25 @@
         <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="F60" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="G60" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H60" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I60" t="n">
-        <v>530.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J60" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K60" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L60" t="s">
         <v>23</v>
@@ -3322,13 +3340,13 @@
         <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="F61" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="G61" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H61" t="n">
         <v>0.10000000149011612</v>
@@ -3337,10 +3355,10 @@
         <v>530.0</v>
       </c>
       <c r="J61" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K61" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L61" t="s">
         <v>23</v>
@@ -3360,25 +3378,25 @@
         <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="F62" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="G62" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H62" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I62" t="n">
-        <v>510.0</v>
+        <v>3180.0</v>
       </c>
       <c r="J62" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K62" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L62" t="s">
         <v>23</v>
@@ -3398,25 +3416,25 @@
         <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="F63" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="G63" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H63" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I63" t="n">
-        <v>1000.0</v>
+        <v>860.0</v>
       </c>
       <c r="J63" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K63" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L63" t="s">
         <v>23</v>
@@ -3436,25 +3454,25 @@
         <v>17</v>
       </c>
       <c r="E64" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="F64" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="G64" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H64" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I64" t="n">
-        <v>530.0</v>
+        <v>3090.0</v>
       </c>
       <c r="J64" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K64" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L64" t="s">
         <v>23</v>
@@ -3474,25 +3492,25 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F65" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="G65" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H65" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I65" t="n">
-        <v>3180.0</v>
+        <v>540.0</v>
       </c>
       <c r="J65" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K65" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L65" t="s">
         <v>23</v>
@@ -3512,25 +3530,25 @@
         <v>17</v>
       </c>
       <c r="E66" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="F66" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="G66" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H66" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I66" t="n">
-        <v>860.0</v>
+        <v>140.0</v>
       </c>
       <c r="J66" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K66" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L66" t="s">
         <v>23</v>
@@ -3550,25 +3568,25 @@
         <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="F67" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="G67" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H67" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I67" t="n">
-        <v>3090.0</v>
+        <v>16570.0</v>
       </c>
       <c r="J67" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K67" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L67" t="s">
         <v>23</v>
@@ -3588,25 +3606,25 @@
         <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="F68" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="G68" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H68" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I68" t="n">
-        <v>540.0</v>
+        <v>3530.0</v>
       </c>
       <c r="J68" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K68" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L68" t="s">
         <v>23</v>
@@ -3626,25 +3644,25 @@
         <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="F69" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="G69" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H69" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I69" t="n">
-        <v>140.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J69" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K69" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L69" t="s">
         <v>23</v>
@@ -3664,25 +3682,25 @@
         <v>17</v>
       </c>
       <c r="E70" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="F70" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="G70" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="H70" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I70" t="n">
-        <v>16570.0</v>
+        <v>725.0</v>
       </c>
       <c r="J70" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K70" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L70" t="s">
         <v>23</v>
@@ -3702,25 +3720,25 @@
         <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="F71" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="G71" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="H71" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I71" t="n">
-        <v>3530.0</v>
+        <v>1520.0</v>
       </c>
       <c r="J71" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K71" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L71" t="s">
         <v>23</v>
@@ -3740,25 +3758,25 @@
         <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="F72" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G72" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H72" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I72" t="n">
-        <v>1000.0</v>
+        <v>4000.0</v>
       </c>
       <c r="J72" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K72" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L72" t="s">
         <v>23</v>
@@ -3778,25 +3796,25 @@
         <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="F73" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="G73" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H73" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I73" t="n">
-        <v>725.0</v>
+        <v>560.0</v>
       </c>
       <c r="J73" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K73" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L73" t="s">
         <v>23</v>
@@ -3816,25 +3834,25 @@
         <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="F74" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="G74" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H74" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I74" t="n">
-        <v>1520.0</v>
+        <v>630.0</v>
       </c>
       <c r="J74" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K74" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L74" t="s">
         <v>23</v>
@@ -3854,25 +3872,25 @@
         <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="F75" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="G75" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H75" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I75" t="n">
-        <v>4000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J75" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K75" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L75" t="s">
         <v>23</v>
@@ -3892,25 +3910,25 @@
         <v>17</v>
       </c>
       <c r="E76" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="F76" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="G76" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H76" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I76" t="n">
-        <v>560.0</v>
+        <v>5000.0</v>
       </c>
       <c r="J76" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K76" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L76" t="s">
         <v>23</v>
@@ -3930,25 +3948,25 @@
         <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="F77" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="G77" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H77" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I77" t="n">
-        <v>630.0</v>
+        <v>5520.0</v>
       </c>
       <c r="J77" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K77" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L77" t="s">
         <v>23</v>
@@ -3968,25 +3986,25 @@
         <v>17</v>
       </c>
       <c r="E78" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="F78" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="G78" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H78" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I78" t="n">
-        <v>1000.0</v>
+        <v>3520.0</v>
       </c>
       <c r="J78" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K78" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L78" t="s">
         <v>23</v>
@@ -4006,25 +4024,25 @@
         <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="F79" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="G79" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H79" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I79" t="n">
-        <v>5000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J79" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K79" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L79" t="s">
         <v>23</v>
@@ -4044,25 +4062,25 @@
         <v>17</v>
       </c>
       <c r="E80" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="F80" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="G80" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H80" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I80" t="n">
-        <v>5520.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J80" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K80" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L80" t="s">
         <v>23</v>
@@ -4082,179 +4100,27 @@
         <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="F81" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="G81" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H81" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I81" t="n">
-        <v>3520.0</v>
+        <v>4000.0</v>
       </c>
       <c r="J81" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="K81" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="L81" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s">
-        <v>14</v>
-      </c>
-      <c r="B82" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" t="s">
-        <v>16</v>
-      </c>
-      <c r="D82" t="s">
-        <v>17</v>
-      </c>
-      <c r="E82" t="s">
-        <v>194</v>
-      </c>
-      <c r="F82" t="s">
-        <v>195</v>
-      </c>
-      <c r="G82" t="s">
-        <v>38</v>
-      </c>
-      <c r="H82" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I82" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="J82" t="s">
-        <v>39</v>
-      </c>
-      <c r="K82" t="s">
-        <v>43</v>
-      </c>
-      <c r="L82" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s">
-        <v>14</v>
-      </c>
-      <c r="B83" t="s">
-        <v>15</v>
-      </c>
-      <c r="C83" t="s">
-        <v>16</v>
-      </c>
-      <c r="D83" t="s">
-        <v>17</v>
-      </c>
-      <c r="E83" t="s">
-        <v>196</v>
-      </c>
-      <c r="F83" t="s">
-        <v>197</v>
-      </c>
-      <c r="G83" t="s">
-        <v>38</v>
-      </c>
-      <c r="H83" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I83" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="J83" t="s">
-        <v>39</v>
-      </c>
-      <c r="K83" t="s">
-        <v>43</v>
-      </c>
-      <c r="L83" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>14</v>
-      </c>
-      <c r="B84" t="s">
-        <v>15</v>
-      </c>
-      <c r="C84" t="s">
-        <v>16</v>
-      </c>
-      <c r="D84" t="s">
-        <v>17</v>
-      </c>
-      <c r="E84" t="s">
-        <v>198</v>
-      </c>
-      <c r="F84" t="s">
-        <v>199</v>
-      </c>
-      <c r="G84" t="s">
-        <v>38</v>
-      </c>
-      <c r="H84" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I84" t="n">
-        <v>4000.0</v>
-      </c>
-      <c r="J84" t="s">
-        <v>39</v>
-      </c>
-      <c r="K84" t="s">
-        <v>43</v>
-      </c>
-      <c r="L84" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>14</v>
-      </c>
-      <c r="B85" t="s">
-        <v>15</v>
-      </c>
-      <c r="C85" t="s">
-        <v>16</v>
-      </c>
-      <c r="D85" t="s">
-        <v>17</v>
-      </c>
-      <c r="E85" t="s">
-        <v>198</v>
-      </c>
-      <c r="F85" t="s">
-        <v>199</v>
-      </c>
-      <c r="G85" t="s">
-        <v>38</v>
-      </c>
-      <c r="H85" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I85" t="n">
-        <v>4000.0</v>
-      </c>
-      <c r="J85" t="s">
-        <v>39</v>
-      </c>
-      <c r="K85" t="s">
-        <v>43</v>
-      </c>
-      <c r="L85" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix width : @media (min-width:1300px){.container{width:1295px}, update PPT file
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/tempxls/개발테스트.xlsx
+++ b/src/main/webapp/resources/tempxls/개발테스트.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="204">
   <si>
     <t>LGIT P/N</t>
   </si>
@@ -83,322 +83,316 @@
     <t>출고시험용</t>
   </si>
   <si>
-    <t>AAAdSLDKJF</t>
-  </si>
-  <si>
-    <t>GLKLVNBDM</t>
-  </si>
-  <si>
-    <t>ei399</t>
-  </si>
-  <si>
-    <t>창고앞</t>
-  </si>
-  <si>
-    <t>!@$-011</t>
+    <t>2CAC01209A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H2R0BA01</t>
+  </si>
+  <si>
+    <t>MURATA ELEKTRONIK</t>
+  </si>
+  <si>
+    <t>A23</t>
+  </si>
+  <si>
+    <t>392+2</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>TESTPRJA1</t>
-  </si>
-  <si>
-    <t>TESTPRJA2</t>
-  </si>
-  <si>
-    <t>TESTPRJA3</t>
-  </si>
-  <si>
-    <t>창고뒤A</t>
-  </si>
-  <si>
-    <t>GESS</t>
-  </si>
-  <si>
-    <t>AGAINEESS</t>
-  </si>
-  <si>
-    <t>MNAJH</t>
-  </si>
-  <si>
-    <t>399fdkAA</t>
-  </si>
-  <si>
-    <t>3층A사이드</t>
-  </si>
-  <si>
-    <t>GDFWEF</t>
-  </si>
-  <si>
-    <t>AGAINNEWAA</t>
-  </si>
-  <si>
-    <t>39fjdn2AA</t>
-  </si>
-  <si>
-    <t>MMGG</t>
-  </si>
-  <si>
-    <t>L432</t>
-  </si>
-  <si>
-    <t>GGEE</t>
-  </si>
-  <si>
-    <t>NEWEXCELIM</t>
-  </si>
-  <si>
-    <t>Hdidlfkje</t>
-  </si>
-  <si>
-    <t>384+2124</t>
-  </si>
-  <si>
-    <t>LG19281NN</t>
-  </si>
-  <si>
-    <t>Desdkfkdfjk</t>
-  </si>
-  <si>
-    <t>MMMMAAAAABB</t>
-  </si>
-  <si>
-    <t>loapdlkj111</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>2255+-9</t>
-  </si>
-  <si>
-    <t>2CAC01209A</t>
-  </si>
-  <si>
-    <t>GRM0335C1H2R0BA01</t>
-  </si>
-  <si>
-    <t>MURATA ELEKTRONIK</t>
+    <t>2CAC01231A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H2R5BA01</t>
+  </si>
+  <si>
+    <t>B39</t>
+  </si>
+  <si>
+    <t>398-25</t>
+  </si>
+  <si>
+    <t>2CAC01187A</t>
+  </si>
+  <si>
+    <t>GRM0335C1HR60WA01</t>
+  </si>
+  <si>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>20+-20</t>
+  </si>
+  <si>
+    <t>2LL2N7BA11K-H</t>
+  </si>
+  <si>
+    <t>LQP03TN2N7B02D</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>392+1</t>
+  </si>
+  <si>
+    <t>2DIT00095A</t>
+  </si>
+  <si>
+    <t>VCUT05E1-SD0</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>2FTZ00032A</t>
+  </si>
+  <si>
+    <t>HHM22106B1</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>A98</t>
+  </si>
+  <si>
+    <t>2FTS00068A</t>
+  </si>
+  <si>
+    <t>SAWFD1G84BH0F0A</t>
+  </si>
+  <si>
+    <t>X298</t>
+  </si>
+  <si>
+    <t>2LL3N4BA11K-R</t>
+  </si>
+  <si>
+    <t>LQP03TN3N4B02D</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>2ICL00079A</t>
+  </si>
+  <si>
+    <t>SKY77767</t>
+  </si>
+  <si>
+    <t>SKYWORKS SOLUTIONS</t>
+  </si>
+  <si>
+    <t>A-A2</t>
+  </si>
+  <si>
+    <t>2FTS00065A</t>
+  </si>
+  <si>
+    <t>F6QA2G535H2JG</t>
+  </si>
+  <si>
+    <t>TAIYO YUDEN</t>
+  </si>
+  <si>
+    <t>B3-31</t>
+  </si>
+  <si>
+    <t>391-21</t>
+  </si>
+  <si>
+    <t>2FTS00064A</t>
+  </si>
+  <si>
+    <t>F6QG2G655P2KE</t>
+  </si>
+  <si>
+    <t>F5-21</t>
+  </si>
+  <si>
+    <t>2FTD00027A</t>
+  </si>
+  <si>
+    <t>D6HN2G655BN59C</t>
+  </si>
+  <si>
+    <t>F4-22</t>
+  </si>
+  <si>
+    <t>298+-1</t>
+  </si>
+  <si>
+    <t>2CAC00828A</t>
+  </si>
+  <si>
+    <t>GRM0335C1E8R0BA01D</t>
+  </si>
+  <si>
+    <t>F3-12</t>
+  </si>
+  <si>
+    <t>29+23</t>
+  </si>
+  <si>
+    <t>2FTS00099A</t>
+  </si>
+  <si>
+    <t>F5QA806M0M2QE</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>2FTS00098A</t>
+  </si>
+  <si>
+    <t>SAYFH806MCA0F1B</t>
+  </si>
+  <si>
+    <t>bv</t>
+  </si>
+  <si>
+    <t>2FTS00097A</t>
+  </si>
+  <si>
+    <t>F5QA847M0M2QR</t>
+  </si>
+  <si>
+    <t>k81</t>
+  </si>
+  <si>
+    <t>2ICL00157A</t>
+  </si>
+  <si>
+    <t>SKY77736</t>
+  </si>
+  <si>
+    <t>공장앞A1</t>
+  </si>
+  <si>
+    <t>2CAC01046A</t>
+  </si>
+  <si>
+    <t>GRM0335C1E1R0BA01D</t>
+  </si>
+  <si>
+    <t>공장앞A2</t>
+  </si>
+  <si>
+    <t>2CAC01039A</t>
+  </si>
+  <si>
+    <t>GRM0335C1E3R3BA01D</t>
+  </si>
+  <si>
+    <t>공장앞A3</t>
+  </si>
+  <si>
+    <t>2LL9N1HA11K-R</t>
+  </si>
+  <si>
+    <t>LQP03TN9N1H02D</t>
+  </si>
+  <si>
+    <t>공장앞A4</t>
+  </si>
+  <si>
+    <t>2RSC01181A</t>
+  </si>
+  <si>
+    <t>RK73H1HTTC6191F</t>
+  </si>
+  <si>
+    <t>KOA CORPORATION NAGANO</t>
+  </si>
+  <si>
+    <t>2FTC00144A</t>
+  </si>
+  <si>
+    <t>DLU-1608-25GS1-A2-AT</t>
+  </si>
+  <si>
+    <t>MAGLAYERS</t>
+  </si>
+  <si>
+    <t>공장앞</t>
+  </si>
+  <si>
+    <t>2FTP00015A</t>
+  </si>
+  <si>
+    <t>DPX165950DT-8126A1</t>
+  </si>
+  <si>
+    <t>A-39</t>
+  </si>
+  <si>
+    <t>2ICZ00186A</t>
+  </si>
+  <si>
+    <t>RFFM8800TR7</t>
+  </si>
+  <si>
+    <t>RFMD</t>
+  </si>
+  <si>
+    <t>A029</t>
+  </si>
+  <si>
+    <t>2ICT00113A</t>
+  </si>
+  <si>
+    <t>AR6003XBC2B-R</t>
+  </si>
+  <si>
+    <t>QUALCOMM INCORPORATED</t>
+  </si>
+  <si>
+    <t>B029</t>
+  </si>
+  <si>
+    <t>2OSR00012A</t>
+  </si>
+  <si>
+    <t>1ZCL26000AB0F</t>
+  </si>
+  <si>
+    <t>KDS</t>
+  </si>
+  <si>
+    <t>B28</t>
+  </si>
+  <si>
+    <t>2CAC00801A</t>
+  </si>
+  <si>
+    <t>GRM033R71E471KA01D</t>
+  </si>
+  <si>
+    <t>BV19</t>
+  </si>
+  <si>
+    <t>2CAC00926A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H6R2BA01D</t>
+  </si>
+  <si>
+    <t>B1982</t>
+  </si>
+  <si>
+    <t>2CAC00824A</t>
+  </si>
+  <si>
+    <t>GRM0335C1H2R2BA01D</t>
   </si>
   <si>
     <t>S1</t>
-  </si>
-  <si>
-    <t>5,435</t>
-  </si>
-  <si>
-    <t>2CAC01231A</t>
-  </si>
-  <si>
-    <t>GRM0335C1H2R5BA01</t>
-  </si>
-  <si>
-    <t>GGGE</t>
-  </si>
-  <si>
-    <t>2CAC01187A</t>
-  </si>
-  <si>
-    <t>GRM0335C1HR60WA01</t>
-  </si>
-  <si>
-    <t>G122</t>
-  </si>
-  <si>
-    <t>2LL2N7BA11K-H</t>
-  </si>
-  <si>
-    <t>LQP03TN2N7B02D</t>
-  </si>
-  <si>
-    <t>G555</t>
-  </si>
-  <si>
-    <t>2DIT00095A</t>
-  </si>
-  <si>
-    <t>VCUT05E1-SD0</t>
-  </si>
-  <si>
-    <t>Vishay</t>
-  </si>
-  <si>
-    <t>20+-20</t>
-  </si>
-  <si>
-    <t>2FTZ00032A</t>
-  </si>
-  <si>
-    <t>HHM22106B1</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>2FTS00068A</t>
-  </si>
-  <si>
-    <t>SAWFD1G84BH0F0A</t>
-  </si>
-  <si>
-    <t>20+-2011</t>
-  </si>
-  <si>
-    <t>2LL3N4BA11K-R</t>
-  </si>
-  <si>
-    <t>LQP03TN3N4B02D</t>
-  </si>
-  <si>
-    <t>2ICL00079A</t>
-  </si>
-  <si>
-    <t>SKY77767</t>
-  </si>
-  <si>
-    <t>SKYWORKS SOLUTIONS</t>
-  </si>
-  <si>
-    <t>2FTS00065A</t>
-  </si>
-  <si>
-    <t>F6QA2G535H2JG</t>
-  </si>
-  <si>
-    <t>TAIYO YUDEN</t>
-  </si>
-  <si>
-    <t>2FTS00064A</t>
-  </si>
-  <si>
-    <t>F6QG2G655P2KE</t>
-  </si>
-  <si>
-    <t>2FTD00027A</t>
-  </si>
-  <si>
-    <t>D6HN2G655BN59C</t>
-  </si>
-  <si>
-    <t>2CAC00828A</t>
-  </si>
-  <si>
-    <t>GRM0335C1E8R0BA01D</t>
-  </si>
-  <si>
-    <t>2FTS00099A</t>
-  </si>
-  <si>
-    <t>F5QA806M0M2QE</t>
-  </si>
-  <si>
-    <t>2FTS00098A</t>
-  </si>
-  <si>
-    <t>SAYFH806MCA0F1B</t>
-  </si>
-  <si>
-    <t>2FTS00097A</t>
-  </si>
-  <si>
-    <t>F5QA847M0M2QR</t>
-  </si>
-  <si>
-    <t>2ICL00157A</t>
-  </si>
-  <si>
-    <t>SKY77736</t>
-  </si>
-  <si>
-    <t>2CAC01046A</t>
-  </si>
-  <si>
-    <t>GRM0335C1E1R0BA01D</t>
-  </si>
-  <si>
-    <t>2CAC01039A</t>
-  </si>
-  <si>
-    <t>GRM0335C1E3R3BA01D</t>
-  </si>
-  <si>
-    <t>2LL9N1HA11K-R</t>
-  </si>
-  <si>
-    <t>LQP03TN9N1H02D</t>
-  </si>
-  <si>
-    <t>2RSC01181A</t>
-  </si>
-  <si>
-    <t>RK73H1HTTC6191F</t>
-  </si>
-  <si>
-    <t>KOA CORPORATION NAGANO</t>
-  </si>
-  <si>
-    <t>2FTC00144A</t>
-  </si>
-  <si>
-    <t>DLU-1608-25GS1-A2-AT</t>
-  </si>
-  <si>
-    <t>MAGLAYERS</t>
-  </si>
-  <si>
-    <t>2FTP00015A</t>
-  </si>
-  <si>
-    <t>DPX165950DT-8126A1</t>
-  </si>
-  <si>
-    <t>2ICZ00186A</t>
-  </si>
-  <si>
-    <t>RFFM8800TR7</t>
-  </si>
-  <si>
-    <t>RFMD</t>
-  </si>
-  <si>
-    <t>2ICT00113A</t>
-  </si>
-  <si>
-    <t>AR6003XBC2B-R</t>
-  </si>
-  <si>
-    <t>QUALCOMM INCORPORATED</t>
-  </si>
-  <si>
-    <t>2OSR00012A</t>
-  </si>
-  <si>
-    <t>1ZCL26000AB0F</t>
-  </si>
-  <si>
-    <t>KDS</t>
-  </si>
-  <si>
-    <t>2CAC00801A</t>
-  </si>
-  <si>
-    <t>GRM033R71E471KA01D</t>
-  </si>
-  <si>
-    <t>2CAC00926A</t>
-  </si>
-  <si>
-    <t>GRM0335C1H6R2BA01D</t>
-  </si>
-  <si>
-    <t>2CAC00824A</t>
-  </si>
-  <si>
-    <t>GRM0335C1H2R2BA01D</t>
   </si>
   <si>
     <t>2FTS00062A</t>
@@ -1221,10 +1215,10 @@
         <v>20</v>
       </c>
       <c r="H5" t="n">
-        <v>54.540000915527344</v>
+        <v>1.1230000257492065</v>
       </c>
       <c r="I5" t="n">
-        <v>998.0</v>
+        <v>128.0</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -1256,19 +1250,19 @@
         <v>25</v>
       </c>
       <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="n">
+        <v>23.11199951171875</v>
+      </c>
+      <c r="I6" t="n">
+        <v>97146.0</v>
+      </c>
+      <c r="J6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" t="n">
-        <v>23.239999771118164</v>
-      </c>
-      <c r="I6" t="n">
-        <v>997.0</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>27</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
       </c>
       <c r="L6" t="s">
         <v>23</v>
@@ -1288,25 +1282,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="n">
+        <v>12.220000267028809</v>
+      </c>
+      <c r="I7" t="n">
+        <v>9937.0</v>
+      </c>
+      <c r="J7" t="s">
         <v>30</v>
       </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" t="n">
-        <v>21.547000885009766</v>
-      </c>
-      <c r="I7" t="n">
-        <v>888.0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
@@ -1326,25 +1320,25 @@
         <v>17</v>
       </c>
       <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.112299919128418</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1934.0</v>
+      </c>
+      <c r="J8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" t="s">
+      <c r="K8" t="s">
         <v>35</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" t="n">
-        <v>123457.0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>88.0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" t="s">
-        <v>38</v>
       </c>
       <c r="L8" t="s">
         <v>23</v>
@@ -1364,25 +1358,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6.341000080108643</v>
+      </c>
+      <c r="I9" t="n">
+        <v>12480.0</v>
+      </c>
+      <c r="J9" t="s">
         <v>39</v>
       </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" t="n">
-        <v>123456.0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>77.0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>37</v>
-      </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="L9" t="s">
         <v>23</v>
@@ -1402,25 +1396,25 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
         <v>42</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="n">
+        <v>3.619999885559082</v>
+      </c>
+      <c r="I10" t="n">
+        <v>508.0</v>
+      </c>
+      <c r="J10" t="s">
         <v>43</v>
       </c>
-      <c r="G10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" t="n">
-        <v>5.656400203704834</v>
-      </c>
-      <c r="I10" t="n">
-        <v>789.0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
       <c r="K10" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>
@@ -1440,25 +1434,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="H11" t="n">
-        <v>77.0</v>
+        <v>12.319999694824219</v>
       </c>
       <c r="I11" t="n">
-        <v>123.0</v>
+        <v>4247.0</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K11" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="L11" t="s">
         <v>23</v>
@@ -1478,25 +1472,25 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="n">
+        <v>54.20000076293945</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2930.0</v>
+      </c>
+      <c r="J12" t="s">
         <v>49</v>
       </c>
-      <c r="F12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" t="n">
-        <v>88.0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>150.0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>52</v>
-      </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="L12" t="s">
         <v>23</v>
@@ -1516,25 +1510,25 @@
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H13" t="n">
-        <v>99.0</v>
+        <v>1235.0</v>
       </c>
       <c r="I13" t="n">
-        <v>97545.0</v>
+        <v>2200.0</v>
       </c>
       <c r="J13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K13" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="L13" t="s">
         <v>23</v>
@@ -1554,25 +1548,25 @@
         <v>17</v>
       </c>
       <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" t="n">
+        <v>24.124000549316406</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2127.0</v>
+      </c>
+      <c r="J14" t="s">
         <v>57</v>
       </c>
-      <c r="F14" t="s">
+      <c r="K14" t="s">
         <v>58</v>
-      </c>
-      <c r="G14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>9975.0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K14" t="s">
-        <v>59</v>
       </c>
       <c r="L14" t="s">
         <v>23</v>
@@ -1592,25 +1586,25 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
         <v>60</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.1230000257492065</v>
+      </c>
+      <c r="I15" t="n">
+        <v>2170.0</v>
+      </c>
+      <c r="J15" t="s">
         <v>61</v>
       </c>
-      <c r="G15" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I15" t="n">
-        <v>1934.0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>52</v>
-      </c>
       <c r="K15" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="L15" t="s">
         <v>23</v>
@@ -1630,25 +1624,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
         <v>63</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" t="n">
+        <v>12.510000228881836</v>
+      </c>
+      <c r="I16" t="n">
+        <v>2180.0</v>
+      </c>
+      <c r="J16" t="s">
         <v>64</v>
       </c>
-      <c r="G16" t="s">
+      <c r="K16" t="s">
         <v>65</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I16" t="n">
-        <v>12600.0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16" t="s">
-        <v>66</v>
       </c>
       <c r="L16" t="s">
         <v>23</v>
@@ -1668,25 +1662,25 @@
         <v>17</v>
       </c>
       <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" t="s">
         <v>67</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.2300000190734863</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1670.0</v>
+      </c>
+      <c r="J17" t="s">
         <v>68</v>
       </c>
-      <c r="G17" t="s">
+      <c r="K17" t="s">
         <v>69</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I17" t="n">
-        <v>510.0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>52</v>
-      </c>
-      <c r="K17" t="s">
-        <v>66</v>
       </c>
       <c r="L17" t="s">
         <v>23</v>
@@ -1712,19 +1706,19 @@
         <v>71</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H18" t="n">
-        <v>0.10000000149011612</v>
+        <v>5.352519989013672</v>
       </c>
       <c r="I18" t="n">
-        <v>4247.0</v>
+        <v>1712.0</v>
       </c>
       <c r="J18" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="K18" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="L18" t="s">
         <v>23</v>
@@ -1750,19 +1744,19 @@
         <v>74</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H19" t="n">
-        <v>0.10000000149011612</v>
+        <v>12.121999740600586</v>
       </c>
       <c r="I19" t="n">
-        <v>2930.0</v>
+        <v>1680.0</v>
       </c>
       <c r="J19" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="K19" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
@@ -1782,25 +1776,25 @@
         <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H20" t="n">
-        <v>0.10000000149011612</v>
+        <v>8.859999656677246</v>
       </c>
       <c r="I20" t="n">
-        <v>2200.0</v>
+        <v>1610.0</v>
       </c>
       <c r="J20" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="K20" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L20" t="s">
         <v>23</v>
@@ -1820,25 +1814,25 @@
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="H21" t="n">
-        <v>0.10000000149011612</v>
+        <v>55.31999969482422</v>
       </c>
       <c r="I21" t="n">
-        <v>2127.0</v>
+        <v>1650.0</v>
       </c>
       <c r="J21" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="K21" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
@@ -1858,25 +1852,25 @@
         <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H22" t="n">
-        <v>0.10000000149011612</v>
+        <v>2.359999895095825</v>
       </c>
       <c r="I22" t="n">
-        <v>2170.0</v>
+        <v>3660.0</v>
       </c>
       <c r="J22" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="K22" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L22" t="s">
         <v>23</v>
@@ -1896,25 +1890,25 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H23" t="n">
-        <v>0.10000000149011612</v>
+        <v>7.53000020980835</v>
       </c>
       <c r="I23" t="n">
-        <v>2180.0</v>
+        <v>3790.0</v>
       </c>
       <c r="J23" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="K23" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
@@ -1934,25 +1928,25 @@
         <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G24" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H24" t="n">
-        <v>0.10000000149011612</v>
+        <v>7.420000076293945</v>
       </c>
       <c r="I24" t="n">
-        <v>1670.0</v>
+        <v>4300.0</v>
       </c>
       <c r="J24" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="K24" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L24" t="s">
         <v>23</v>
@@ -1972,25 +1966,25 @@
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G25" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="H25" t="n">
-        <v>0.10000000149011612</v>
+        <v>4.320000171661377</v>
       </c>
       <c r="I25" t="n">
-        <v>1712.0</v>
+        <v>8980.0</v>
       </c>
       <c r="J25" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="K25" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L25" t="s">
         <v>23</v>
@@ -2010,25 +2004,25 @@
         <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="G26" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="H26" t="n">
-        <v>0.10000000149011612</v>
+        <v>52.5</v>
       </c>
       <c r="I26" t="n">
-        <v>1680.0</v>
+        <v>4480.0</v>
       </c>
       <c r="J26" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="K26" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L26" t="s">
         <v>23</v>
@@ -2048,25 +2042,25 @@
         <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="F27" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="G27" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="H27" t="n">
-        <v>0.10000000149011612</v>
+        <v>45.20000076293945</v>
       </c>
       <c r="I27" t="n">
-        <v>1610.0</v>
+        <v>2260.0</v>
       </c>
       <c r="J27" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="K27" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L27" t="s">
         <v>23</v>
@@ -2086,25 +2080,25 @@
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G28" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="H28" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I28" t="n">
-        <v>1650.0</v>
+        <v>768.0</v>
       </c>
       <c r="J28" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="K28" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L28" t="s">
         <v>23</v>
@@ -2124,25 +2118,25 @@
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="F29" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G29" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="H29" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I29" t="n">
-        <v>3660.0</v>
+        <v>1275.0</v>
       </c>
       <c r="J29" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="K29" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L29" t="s">
         <v>23</v>
@@ -2162,25 +2156,25 @@
         <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="F30" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="G30" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="H30" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I30" t="n">
-        <v>3790.0</v>
+        <v>2200.0</v>
       </c>
       <c r="J30" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="K30" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L30" t="s">
         <v>23</v>
@@ -2200,25 +2194,25 @@
         <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H31" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I31" t="n">
-        <v>4300.0</v>
+        <v>1560.0</v>
       </c>
       <c r="J31" t="s">
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="K31" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L31" t="s">
         <v>23</v>
@@ -2238,25 +2232,25 @@
         <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="F32" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="G32" t="s">
-        <v>103</v>
+        <v>20</v>
       </c>
       <c r="H32" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I32" t="n">
-        <v>8980.0</v>
+        <v>1330.0</v>
       </c>
       <c r="J32" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="K32" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L32" t="s">
         <v>23</v>
@@ -2276,25 +2270,25 @@
         <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="F33" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="G33" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="H33" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I33" t="n">
-        <v>4447.0</v>
+        <v>1330.0</v>
       </c>
       <c r="J33" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K33" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L33" t="s">
         <v>23</v>
@@ -2314,25 +2308,25 @@
         <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="F34" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="G34" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="H34" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I34" t="n">
-        <v>2260.0</v>
+        <v>1020.0</v>
       </c>
       <c r="J34" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K34" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L34" t="s">
         <v>23</v>
@@ -2352,25 +2346,25 @@
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="F35" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="G35" t="s">
-        <v>111</v>
+        <v>20</v>
       </c>
       <c r="H35" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I35" t="n">
-        <v>768.0</v>
+        <v>15830.0</v>
       </c>
       <c r="J35" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K35" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L35" t="s">
         <v>23</v>
@@ -2390,25 +2384,25 @@
         <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="F36" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="G36" t="s">
-        <v>114</v>
+        <v>52</v>
       </c>
       <c r="H36" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I36" t="n">
-        <v>1275.0</v>
+        <v>500.0</v>
       </c>
       <c r="J36" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K36" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L36" t="s">
         <v>23</v>
@@ -2428,25 +2422,25 @@
         <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="F37" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="G37" t="s">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="H37" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I37" t="n">
-        <v>2200.0</v>
+        <v>19.0</v>
       </c>
       <c r="J37" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K37" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L37" t="s">
         <v>23</v>
@@ -2466,25 +2460,25 @@
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H38" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I38" t="n">
-        <v>1560.0</v>
+        <v>2710.0</v>
       </c>
       <c r="J38" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K38" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L38" t="s">
         <v>23</v>
@@ -2504,25 +2498,25 @@
         <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="F39" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G39" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H39" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I39" t="n">
-        <v>1330.0</v>
+        <v>187.0</v>
       </c>
       <c r="J39" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K39" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L39" t="s">
         <v>23</v>
@@ -2542,25 +2536,25 @@
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="F40" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="G40" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H40" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I40" t="n">
-        <v>1330.0</v>
+        <v>680.0</v>
       </c>
       <c r="J40" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K40" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L40" t="s">
         <v>23</v>
@@ -2580,25 +2574,25 @@
         <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="F41" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="G41" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="H41" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I41" t="n">
-        <v>1020.0</v>
+        <v>72.0</v>
       </c>
       <c r="J41" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K41" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L41" t="s">
         <v>23</v>
@@ -2618,25 +2612,25 @@
         <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="F42" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="G42" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H42" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I42" t="n">
-        <v>15830.0</v>
+        <v>4060.0</v>
       </c>
       <c r="J42" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K42" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L42" t="s">
         <v>23</v>
@@ -2656,25 +2650,25 @@
         <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="F43" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="G43" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="H43" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I43" t="n">
-        <v>500.0</v>
+        <v>520.0</v>
       </c>
       <c r="J43" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K43" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L43" t="s">
         <v>23</v>
@@ -2694,25 +2688,25 @@
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F44" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="G44" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H44" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I44" t="n">
-        <v>19.0</v>
+        <v>520.0</v>
       </c>
       <c r="J44" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K44" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L44" t="s">
         <v>23</v>
@@ -2732,25 +2726,25 @@
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="F45" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="G45" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H45" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I45" t="n">
-        <v>2710.0</v>
+        <v>3300.0</v>
       </c>
       <c r="J45" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K45" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L45" t="s">
         <v>23</v>
@@ -2770,25 +2764,25 @@
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="F46" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="G46" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H46" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I46" t="n">
-        <v>187.0</v>
+        <v>530.0</v>
       </c>
       <c r="J46" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K46" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L46" t="s">
         <v>23</v>
@@ -2808,25 +2802,25 @@
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="F47" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="G47" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H47" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I47" t="n">
-        <v>680.0</v>
+        <v>1270.0</v>
       </c>
       <c r="J47" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K47" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L47" t="s">
         <v>23</v>
@@ -2846,25 +2840,25 @@
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="F48" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="G48" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H48" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I48" t="n">
-        <v>72.0</v>
+        <v>1430.0</v>
       </c>
       <c r="J48" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K48" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L48" t="s">
         <v>23</v>
@@ -2884,25 +2878,25 @@
         <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="F49" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="G49" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H49" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I49" t="n">
-        <v>4060.0</v>
+        <v>480.0</v>
       </c>
       <c r="J49" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K49" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L49" t="s">
         <v>23</v>
@@ -2922,25 +2916,25 @@
         <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="F50" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="G50" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H50" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I50" t="n">
-        <v>520.0</v>
+        <v>530.0</v>
       </c>
       <c r="J50" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K50" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L50" t="s">
         <v>23</v>
@@ -2960,25 +2954,25 @@
         <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="F51" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="G51" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H51" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I51" t="n">
-        <v>520.0</v>
+        <v>530.0</v>
       </c>
       <c r="J51" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K51" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L51" t="s">
         <v>23</v>
@@ -2998,25 +2992,25 @@
         <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="F52" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="G52" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H52" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I52" t="n">
-        <v>3300.0</v>
+        <v>510.0</v>
       </c>
       <c r="J52" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K52" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L52" t="s">
         <v>23</v>
@@ -3036,25 +3030,25 @@
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="F53" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G53" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H53" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I53" t="n">
-        <v>530.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J53" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K53" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L53" t="s">
         <v>23</v>
@@ -3074,25 +3068,25 @@
         <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="F54" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="G54" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H54" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I54" t="n">
-        <v>1270.0</v>
+        <v>530.0</v>
       </c>
       <c r="J54" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K54" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L54" t="s">
         <v>23</v>
@@ -3112,25 +3106,25 @@
         <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="F55" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="G55" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H55" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I55" t="n">
-        <v>1430.0</v>
+        <v>3180.0</v>
       </c>
       <c r="J55" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K55" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L55" t="s">
         <v>23</v>
@@ -3150,25 +3144,25 @@
         <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="F56" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="G56" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H56" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I56" t="n">
-        <v>480.0</v>
+        <v>860.0</v>
       </c>
       <c r="J56" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K56" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L56" t="s">
         <v>23</v>
@@ -3188,25 +3182,25 @@
         <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="F57" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="G57" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H57" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I57" t="n">
-        <v>530.0</v>
+        <v>3090.0</v>
       </c>
       <c r="J57" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K57" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L57" t="s">
         <v>23</v>
@@ -3226,25 +3220,25 @@
         <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="F58" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="G58" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H58" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I58" t="n">
-        <v>530.0</v>
+        <v>540.0</v>
       </c>
       <c r="J58" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K58" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L58" t="s">
         <v>23</v>
@@ -3264,25 +3258,25 @@
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F59" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="G59" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H59" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I59" t="n">
-        <v>510.0</v>
+        <v>140.0</v>
       </c>
       <c r="J59" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K59" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L59" t="s">
         <v>23</v>
@@ -3302,25 +3296,25 @@
         <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="F60" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="G60" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H60" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I60" t="n">
-        <v>1000.0</v>
+        <v>16570.0</v>
       </c>
       <c r="J60" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K60" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L60" t="s">
         <v>23</v>
@@ -3340,25 +3334,25 @@
         <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="F61" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="G61" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H61" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I61" t="n">
-        <v>530.0</v>
+        <v>3530.0</v>
       </c>
       <c r="J61" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K61" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L61" t="s">
         <v>23</v>
@@ -3378,25 +3372,25 @@
         <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="F62" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="G62" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H62" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I62" t="n">
-        <v>3180.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J62" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K62" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L62" t="s">
         <v>23</v>
@@ -3416,25 +3410,25 @@
         <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="F63" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="G63" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H63" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I63" t="n">
-        <v>860.0</v>
+        <v>725.0</v>
       </c>
       <c r="J63" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K63" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L63" t="s">
         <v>23</v>
@@ -3454,25 +3448,25 @@
         <v>17</v>
       </c>
       <c r="E64" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="F64" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="G64" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H64" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I64" t="n">
-        <v>3090.0</v>
+        <v>1520.0</v>
       </c>
       <c r="J64" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K64" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L64" t="s">
         <v>23</v>
@@ -3492,25 +3486,25 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="F65" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="G65" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H65" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I65" t="n">
-        <v>540.0</v>
+        <v>4000.0</v>
       </c>
       <c r="J65" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K65" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L65" t="s">
         <v>23</v>
@@ -3530,25 +3524,25 @@
         <v>17</v>
       </c>
       <c r="E66" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="F66" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G66" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H66" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I66" t="n">
-        <v>140.0</v>
+        <v>560.0</v>
       </c>
       <c r="J66" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K66" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L66" t="s">
         <v>23</v>
@@ -3568,25 +3562,25 @@
         <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="F67" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="G67" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H67" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I67" t="n">
-        <v>16570.0</v>
+        <v>630.0</v>
       </c>
       <c r="J67" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K67" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L67" t="s">
         <v>23</v>
@@ -3606,25 +3600,25 @@
         <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="F68" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="G68" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H68" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I68" t="n">
-        <v>3530.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J68" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K68" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L68" t="s">
         <v>23</v>
@@ -3644,25 +3638,25 @@
         <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="F69" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="G69" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H69" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I69" t="n">
-        <v>1000.0</v>
+        <v>5000.0</v>
       </c>
       <c r="J69" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K69" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L69" t="s">
         <v>23</v>
@@ -3682,25 +3676,25 @@
         <v>17</v>
       </c>
       <c r="E70" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="F70" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="G70" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="H70" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I70" t="n">
-        <v>725.0</v>
+        <v>5520.0</v>
       </c>
       <c r="J70" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K70" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L70" t="s">
         <v>23</v>
@@ -3720,25 +3714,25 @@
         <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="F71" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="G71" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="H71" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I71" t="n">
-        <v>1520.0</v>
+        <v>3520.0</v>
       </c>
       <c r="J71" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K71" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L71" t="s">
         <v>23</v>
@@ -3758,25 +3752,25 @@
         <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="F72" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="G72" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H72" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I72" t="n">
-        <v>4000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J72" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K72" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L72" t="s">
         <v>23</v>
@@ -3796,25 +3790,25 @@
         <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="F73" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="G73" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H73" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I73" t="n">
-        <v>560.0</v>
+        <v>1000.0</v>
       </c>
       <c r="J73" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K73" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L73" t="s">
         <v>23</v>
@@ -3834,293 +3828,27 @@
         <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="F74" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="G74" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H74" t="n">
         <v>0.10000000149011612</v>
       </c>
       <c r="I74" t="n">
-        <v>630.0</v>
+        <v>4000.0</v>
       </c>
       <c r="J74" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="K74" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="L74" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>14</v>
-      </c>
-      <c r="B75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C75" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75" t="s">
-        <v>17</v>
-      </c>
-      <c r="E75" t="s">
-        <v>192</v>
-      </c>
-      <c r="F75" t="s">
-        <v>193</v>
-      </c>
-      <c r="G75" t="s">
-        <v>51</v>
-      </c>
-      <c r="H75" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I75" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="J75" t="s">
-        <v>52</v>
-      </c>
-      <c r="K75" t="s">
-        <v>66</v>
-      </c>
-      <c r="L75" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>14</v>
-      </c>
-      <c r="B76" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76" t="s">
-        <v>16</v>
-      </c>
-      <c r="D76" t="s">
-        <v>17</v>
-      </c>
-      <c r="E76" t="s">
-        <v>194</v>
-      </c>
-      <c r="F76" t="s">
-        <v>195</v>
-      </c>
-      <c r="G76" t="s">
-        <v>51</v>
-      </c>
-      <c r="H76" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I76" t="n">
-        <v>5000.0</v>
-      </c>
-      <c r="J76" t="s">
-        <v>52</v>
-      </c>
-      <c r="K76" t="s">
-        <v>66</v>
-      </c>
-      <c r="L76" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" t="s">
-        <v>15</v>
-      </c>
-      <c r="C77" t="s">
-        <v>16</v>
-      </c>
-      <c r="D77" t="s">
-        <v>17</v>
-      </c>
-      <c r="E77" t="s">
-        <v>196</v>
-      </c>
-      <c r="F77" t="s">
-        <v>197</v>
-      </c>
-      <c r="G77" t="s">
-        <v>51</v>
-      </c>
-      <c r="H77" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I77" t="n">
-        <v>5520.0</v>
-      </c>
-      <c r="J77" t="s">
-        <v>52</v>
-      </c>
-      <c r="K77" t="s">
-        <v>66</v>
-      </c>
-      <c r="L77" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
-        <v>14</v>
-      </c>
-      <c r="B78" t="s">
-        <v>15</v>
-      </c>
-      <c r="C78" t="s">
-        <v>16</v>
-      </c>
-      <c r="D78" t="s">
-        <v>17</v>
-      </c>
-      <c r="E78" t="s">
-        <v>198</v>
-      </c>
-      <c r="F78" t="s">
-        <v>199</v>
-      </c>
-      <c r="G78" t="s">
-        <v>51</v>
-      </c>
-      <c r="H78" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I78" t="n">
-        <v>3520.0</v>
-      </c>
-      <c r="J78" t="s">
-        <v>52</v>
-      </c>
-      <c r="K78" t="s">
-        <v>66</v>
-      </c>
-      <c r="L78" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s">
-        <v>14</v>
-      </c>
-      <c r="B79" t="s">
-        <v>15</v>
-      </c>
-      <c r="C79" t="s">
-        <v>16</v>
-      </c>
-      <c r="D79" t="s">
-        <v>17</v>
-      </c>
-      <c r="E79" t="s">
-        <v>200</v>
-      </c>
-      <c r="F79" t="s">
-        <v>201</v>
-      </c>
-      <c r="G79" t="s">
-        <v>51</v>
-      </c>
-      <c r="H79" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I79" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="J79" t="s">
-        <v>52</v>
-      </c>
-      <c r="K79" t="s">
-        <v>66</v>
-      </c>
-      <c r="L79" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s">
-        <v>14</v>
-      </c>
-      <c r="B80" t="s">
-        <v>15</v>
-      </c>
-      <c r="C80" t="s">
-        <v>16</v>
-      </c>
-      <c r="D80" t="s">
-        <v>17</v>
-      </c>
-      <c r="E80" t="s">
-        <v>202</v>
-      </c>
-      <c r="F80" t="s">
-        <v>203</v>
-      </c>
-      <c r="G80" t="s">
-        <v>51</v>
-      </c>
-      <c r="H80" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I80" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="J80" t="s">
-        <v>52</v>
-      </c>
-      <c r="K80" t="s">
-        <v>66</v>
-      </c>
-      <c r="L80" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s">
-        <v>14</v>
-      </c>
-      <c r="B81" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D81" t="s">
-        <v>17</v>
-      </c>
-      <c r="E81" t="s">
-        <v>204</v>
-      </c>
-      <c r="F81" t="s">
-        <v>205</v>
-      </c>
-      <c r="G81" t="s">
-        <v>51</v>
-      </c>
-      <c r="H81" t="n">
-        <v>0.10000000149011612</v>
-      </c>
-      <c r="I81" t="n">
-        <v>4000.0</v>
-      </c>
-      <c r="J81" t="s">
-        <v>52</v>
-      </c>
-      <c r="K81" t="s">
-        <v>66</v>
-      </c>
-      <c r="L81" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>